<commit_message>
adding taxonomies to nodes for published webs from rmangal
</commit_message>
<xml_diff>
--- a/Published_webs/rmangal/rmangal_datasets.xlsx
+++ b/Published_webs/rmangal/rmangal_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ana/Dropbox/2020/Dissertation/DNA_predators/Published_webs/rmangal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6E652D-A85A-034B-8D22-08B58FBB4F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6298205D-46DB-714E-9035-5DD3F15A09FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2960" windowWidth="19940" windowHeight="13040" xr2:uid="{867384A0-329A-C447-8C79-A046D35C1604}"/>
+    <workbookView xWindow="120" yWindow="6080" windowWidth="13280" windowHeight="13040" xr2:uid="{867384A0-329A-C447-8C79-A046D35C1604}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -240,6 +240,30 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>web 2 seems useful</t>
+  </si>
+  <si>
+    <t>too aggregated</t>
+  </si>
+  <si>
+    <t>use?</t>
+  </si>
+  <si>
+    <t>4 webs with predation</t>
+  </si>
+  <si>
+    <t>2 webs</t>
+  </si>
+  <si>
+    <t>11 webs, lots of unspecified interactin types</t>
+  </si>
+  <si>
+    <t>2,4,5, 6 have predation</t>
+  </si>
+  <si>
+    <t>aggregated</t>
   </si>
 </sst>
 </file>
@@ -255,12 +279,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -275,8 +305,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,19 +622,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B56BBF-DD0A-554F-8775-2E0C26CD91BD}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G13" sqref="A13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -619,25 +651,37 @@
       <c r="E1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>91</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>99</v>
       </c>
@@ -650,98 +694,136 @@
       <c r="E3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>107</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>114</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>115</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="E6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>117</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>124</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="E8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>126</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>148</v>
       </c>
@@ -757,59 +839,81 @@
       <c r="E10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>151</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="E11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>152</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>154</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>161</v>
       </c>
@@ -825,22 +929,33 @@
       <c r="E14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>178</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>

</xml_diff>